<commit_message>
Dropdown, Button zur Modusänderung
Drop down zur Auswahl der Ui Fenster WarehouseItem und Queue
</commit_message>
<xml_diff>
--- a/Software/Quellen/Quellen Softwareprojekt.xlsx
+++ b/Software/Quellen/Quellen Softwareprojekt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laris\OneDrive\Dokumente\GitHub\digital-commissioning-tool\Software\Quellen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3EDDB3-0E25-4FC2-A97F-5C200B82DBEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D815C9-6BE8-4A51-867C-2D7701D0AA7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B68F1911-A882-4187-85F0-058BBD1A61E8}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Beschreibung</t>
   </si>
@@ -80,6 +80,18 @@
   </si>
   <si>
     <t>Schriftart Timer</t>
+  </si>
+  <si>
+    <t>https://www.clipartmax.com/png/small/330-3306271_wall-icon-clipart-wall-brick-building-wall-icon.png</t>
+  </si>
+  <si>
+    <t>https://www.freeiconspng.com/img/33857</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>08.01.21</t>
   </si>
 </sst>
 </file>
@@ -486,7 +498,7 @@
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,10 +542,26 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C4" s="1"/>
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C5" s="1"/>
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" s="1"/>

</xml_diff>

<commit_message>
MOSIM Button an UI angepasst
</commit_message>
<xml_diff>
--- a/Software/Quellen/Quellen Softwareprojekt.xlsx
+++ b/Software/Quellen/Quellen Softwareprojekt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laris\OneDrive\Dokumente\GitHub\digital-commissioning-tool\Software\Quellen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pascal\Documents\UnityProject\digital-commissioning-tool\Software\Quellen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D815C9-6BE8-4A51-867C-2D7701D0AA7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AF47D6-C117-4B38-A3B2-D3ADF3EEE2DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B68F1911-A882-4187-85F0-058BBD1A61E8}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B68F1911-A882-4187-85F0-058BBD1A61E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Quellen DigCommTool" sheetId="1" r:id="rId1"/>
@@ -64,15 +64,6 @@
     <t>Simple Town Asset</t>
   </si>
   <si>
-    <t>https://www.cgtrader.com/free-3d-models/architectural/door/roller-shutters-rigged-animated</t>
-  </si>
-  <si>
-    <t>3D-Model für Garagentor</t>
-  </si>
-  <si>
-    <t>01.11.20</t>
-  </si>
-  <si>
     <t>https://www.1001fonts.com/led-font.html#gallery</t>
   </si>
   <si>
@@ -92,6 +83,15 @@
   </si>
   <si>
     <t>08.01.21</t>
+  </si>
+  <si>
+    <t>TreeView</t>
+  </si>
+  <si>
+    <t>https://assetstore.unity.com/packages/tools/gui/treeview-control-824</t>
+  </si>
+  <si>
+    <t>03.12.20</t>
   </si>
 </sst>
 </file>
@@ -156,11 +156,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -498,17 +499,17 @@
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="42.88671875" customWidth="1"/>
-    <col min="2" max="2" width="57.33203125" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" customWidth="1"/>
+    <col min="1" max="1" width="42.90625" customWidth="1"/>
+    <col min="2" max="2" width="57.36328125" customWidth="1"/>
+    <col min="3" max="3" width="22.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,192 +520,192 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C53" s="1"/>
     </row>
   </sheetData>
@@ -724,13 +725,13 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="57.33203125" customWidth="1"/>
-    <col min="2" max="2" width="68.6640625" customWidth="1"/>
+    <col min="1" max="1" width="57.36328125" customWidth="1"/>
+    <col min="2" max="2" width="68.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -738,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -746,7 +747,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -754,7 +755,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -762,7 +763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -770,27 +771,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
     </row>

</xml_diff>